<commit_message>
Update BOM, add enclosure and speaker
</commit_message>
<xml_diff>
--- a/bom/door_bell.xlsx
+++ b/bom/door_bell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/espen/Projects/KiCad/projects/dual-button-doorbell/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5438732-510B-6D48-B98E-A5014AABB14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0FA3C2-5781-CA45-8CC8-6266EAE8D663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14320" yWindow="3900" windowWidth="70600" windowHeight="17440" xr2:uid="{3EF4FAFF-71C4-2545-A4EC-35E72D213441}"/>
+    <workbookView xWindow="0" yWindow="1220" windowWidth="33600" windowHeight="17440" xr2:uid="{3EF4FAFF-71C4-2545-A4EC-35E72D213441}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="288">
   <si>
     <t>Ref</t>
   </si>
@@ -767,24 +767,6 @@
     <t>Tactile Switches 50mA 12VDC F065 4.3mm Gull Wing</t>
   </si>
   <si>
-    <t>863-NCP1117ST33T3G</t>
-  </si>
-  <si>
-    <t>NCP1117ST33T3G</t>
-  </si>
-  <si>
-    <t>LDO Voltage Regulators 3.3V 1A Positive</t>
-  </si>
-  <si>
-    <t>863-NCP1117ST50T3G</t>
-  </si>
-  <si>
-    <t>NCP1117ST50T3G</t>
-  </si>
-  <si>
-    <t>LDO Voltage Regulators 5.0V 1A Positive</t>
-  </si>
-  <si>
     <t>700-MAX98357AETE+T</t>
   </si>
   <si>
@@ -858,6 +840,66 @@
   </si>
   <si>
     <t>Bridge Rectifiers Bridge Rectifier HDS</t>
+  </si>
+  <si>
+    <t>637-LDI1117-05H</t>
+  </si>
+  <si>
+    <t>LDI1117-05H</t>
+  </si>
+  <si>
+    <t>Diotec Semiconductor</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulators VR, SOT-223, 20V, 4.95V, 5.05V</t>
+  </si>
+  <si>
+    <t>637-LDI1117-3.3H</t>
+  </si>
+  <si>
+    <t>LDI1117-3.3H</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulators VR, SOT-223, 20V, 3.267V, 3.333V</t>
+  </si>
+  <si>
+    <t>NCP1117-5.0_SOT223</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 5.0V, SOT-223</t>
+  </si>
+  <si>
+    <t>Enclosure</t>
+  </si>
+  <si>
+    <t>789-P1A-303012</t>
+  </si>
+  <si>
+    <t>P1A-303012</t>
+  </si>
+  <si>
+    <t>New Age Enclosures</t>
+  </si>
+  <si>
+    <t>Enclosures, Boxes &amp; Cases Vented Cube</t>
+  </si>
+  <si>
+    <t>Vented enclosure, white</t>
+  </si>
+  <si>
+    <t>490-CES-603318-24PM</t>
+  </si>
+  <si>
+    <t>CES-603318-24PM</t>
+  </si>
+  <si>
+    <t>CUI Devices</t>
+  </si>
+  <si>
+    <t>Speakers &amp; Transducers speaker, 60 x 33mm rectangle, 2W, 4ohm</t>
+  </si>
+  <si>
+    <t>Enclosed speaker, 4ohm, 2W</t>
   </si>
 </sst>
 </file>
@@ -867,7 +909,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;kr&quot;\ * #,##0.00_);_(&quot;kr&quot;\ * \(#,##0.00\);_(&quot;kr&quot;\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -879,6 +921,20 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -904,7 +960,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -914,6 +970,11 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1228,10 +1289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E0BB35-FFD4-EE4A-92C0-E7A191100E0E}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1240,7 +1301,7 @@
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="34.5" customWidth="1"/>
-    <col min="5" max="5" width="86.6640625" customWidth="1"/>
+    <col min="5" max="5" width="94.83203125" customWidth="1"/>
     <col min="6" max="6" width="90.6640625" customWidth="1"/>
     <col min="7" max="7" width="24.1640625" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" customWidth="1"/>
@@ -1284,16 +1345,16 @@
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -1580,16 +1641,16 @@
         <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I8" t="s">
         <v>175</v>
       </c>
       <c r="J8" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="K8" t="s">
         <v>176</v>
@@ -2536,37 +2597,37 @@
         <v>124</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>275</v>
       </c>
       <c r="E31" t="s">
         <v>126</v>
       </c>
       <c r="F31" t="s">
-        <v>127</v>
+        <v>276</v>
       </c>
       <c r="G31" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="I31" t="s">
-        <v>179</v>
+        <v>270</v>
       </c>
       <c r="J31" t="s">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="K31" t="s">
         <v>157</v>
       </c>
       <c r="L31">
-        <v>10</v>
-      </c>
-      <c r="M31" s="3">
-        <v>6.9</v>
-      </c>
-      <c r="N31" s="3">
-        <v>69</v>
+        <v>20</v>
+      </c>
+      <c r="M31" s="5">
+        <v>5.28</v>
+      </c>
+      <c r="N31" s="5">
+        <v>105.6</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -2589,16 +2650,16 @@
         <v>132</v>
       </c>
       <c r="G32" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I32" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="J32" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="K32" t="s">
         <v>157</v>
@@ -2613,7 +2674,7 @@
         <v>156.85</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>133</v>
       </c>
@@ -2632,32 +2693,32 @@
       <c r="F33" t="s">
         <v>127</v>
       </c>
-      <c r="G33" t="s">
-        <v>243</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="I33" t="s">
-        <v>179</v>
-      </c>
-      <c r="J33" t="s">
-        <v>245</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="G33" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="K33" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="6">
         <v>10</v>
       </c>
-      <c r="M33" s="3">
-        <v>6.48</v>
-      </c>
-      <c r="N33" s="3">
-        <v>64.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M33" s="7">
+        <v>5.28</v>
+      </c>
+      <c r="N33" s="7">
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>135</v>
       </c>
@@ -2677,16 +2738,16 @@
         <v>138</v>
       </c>
       <c r="G34" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="I34" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="J34" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="K34" t="s">
         <v>157</v>
@@ -2701,7 +2762,7 @@
         <v>349.44</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>139</v>
       </c>
@@ -2721,16 +2782,16 @@
         <v>142</v>
       </c>
       <c r="G35" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="I35" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J35" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="K35" t="s">
         <v>157</v>
@@ -2745,7 +2806,7 @@
         <v>89.1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -2765,16 +2826,16 @@
         <v>147</v>
       </c>
       <c r="G36" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="I36" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="J36" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="K36" t="s">
         <v>157</v>
@@ -2789,7 +2850,7 @@
         <v>197.05</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>148</v>
       </c>
@@ -2809,16 +2870,16 @@
         <v>151</v>
       </c>
       <c r="G37" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I37" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J37" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="K37" t="s">
         <v>157</v>
@@ -2832,6 +2893,90 @@
       <c r="N37" s="3">
         <v>38.4</v>
       </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>277</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D38" t="s">
+        <v>282</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="G38" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="L38" s="8">
+        <v>2</v>
+      </c>
+      <c r="M38" s="9">
+        <v>47.81</v>
+      </c>
+      <c r="N38" s="9">
+        <v>95.62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D39" t="s">
+        <v>287</v>
+      </c>
+      <c r="G39" t="s">
+        <v>283</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I39" t="s">
+        <v>285</v>
+      </c>
+      <c r="J39" t="s">
+        <v>286</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39" s="2">
+        <v>61.33</v>
+      </c>
+      <c r="N39" s="5">
+        <v>61.33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update BOM to version 1.1
</commit_message>
<xml_diff>
--- a/bom/door_bell.xlsx
+++ b/bom/door_bell.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/espen/Projects/KiCad/projects/dual-button-doorbell/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0FA3C2-5781-CA45-8CC8-6266EAE8D663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8884B0AA-CC99-DC44-AA49-41085B95DBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1220" windowWidth="33600" windowHeight="17440" xr2:uid="{3EF4FAFF-71C4-2545-A4EC-35E72D213441}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="290">
   <si>
     <t>Ref</t>
   </si>
@@ -89,18 +89,12 @@
     <t>Unpolarized capacitor</t>
   </si>
   <si>
-    <t>C2, C13, C14, C18</t>
-  </si>
-  <si>
     <t>C_Decoupling</t>
   </si>
   <si>
     <t>Unpolarized capacitor, small symbol</t>
   </si>
   <si>
-    <t>C3, C7</t>
-  </si>
-  <si>
     <t>220uF</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t>Diode, filled shape</t>
   </si>
   <si>
-    <t>D3, D4, D5, D8, D9, D10, D11</t>
-  </si>
-  <si>
     <t>TVS</t>
   </si>
   <si>
@@ -167,9 +158,6 @@
     <t>Bidirectional transient-voltage-suppression diode, filled shape</t>
   </si>
   <si>
-    <t>D6</t>
-  </si>
-  <si>
     <t>RED</t>
   </si>
   <si>
@@ -353,21 +341,12 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>R3, R4, R5, R6, R7, R10, R15, R16, R17, R18, R19, R20, R21</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
-    <t>R8, R9</t>
-  </si>
-  <si>
     <t>100Ω</t>
   </si>
   <si>
-    <t>R11, R12, R13, R14</t>
-  </si>
-  <si>
     <t>75Ω</t>
   </si>
   <si>
@@ -377,12 +356,6 @@
     <t>100k</t>
   </si>
   <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
     <t>SW_Push</t>
   </si>
   <si>
@@ -392,21 +365,6 @@
     <t>Push button switch, generic, two pins</t>
   </si>
   <si>
-    <t>TP1</t>
-  </si>
-  <si>
-    <t>Ground</t>
-  </si>
-  <si>
-    <t>TestPoint</t>
-  </si>
-  <si>
-    <t>TestPoint:TestPoint_Loop_D3.50mm_Drill0.9mm_Beaded</t>
-  </si>
-  <si>
-    <t>test point</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -900,6 +858,54 @@
   </si>
   <si>
     <t>Enclosed speaker, 4ohm, 2W</t>
+  </si>
+  <si>
+    <t>SW1, SW2</t>
+  </si>
+  <si>
+    <t>Reset,Boot</t>
+  </si>
+  <si>
+    <t>C2, C7</t>
+  </si>
+  <si>
+    <t>C2, C3, C13, C14, C18</t>
+  </si>
+  <si>
+    <t>D4, D5, D6, D9, D10, D11, D12</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>TVSP</t>
+  </si>
+  <si>
+    <t>WE-TVSP Power TVS Diode</t>
+  </si>
+  <si>
+    <t>710-824521131</t>
+  </si>
+  <si>
+    <t>Wurth</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>2,4k</t>
+  </si>
+  <si>
+    <t>R5, R6, R7, R8</t>
+  </si>
+  <si>
+    <t>R11, R12</t>
+  </si>
+  <si>
+    <t>R14, R15, R16, R17</t>
+  </si>
+  <si>
+    <t>R3, R4, R9, R10, R13, R18, R19, R20, R21, R22</t>
   </si>
 </sst>
 </file>
@@ -960,7 +966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -975,6 +981,9 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E0BB35-FFD4-EE4A-92C0-E7A191100E0E}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1333,10 +1342,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -1345,16 +1354,16 @@
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -1377,19 +1386,19 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="I2" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="J2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="K2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L2">
         <v>10</v>
@@ -1421,19 +1430,19 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="I3" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="J3" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="K3" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L3">
         <v>100</v>
@@ -1447,37 +1456,37 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>277</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="I4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="J4" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="K4" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L4">
         <v>100</v>
@@ -1491,37 +1500,37 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>276</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
       <c r="G5" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="I5" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="J5" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="K5" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L5">
         <v>10</v>
@@ -1535,37 +1544,37 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="I6" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="J6" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="K6" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L6">
         <v>100</v>
@@ -1579,13 +1588,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -1597,19 +1606,19 @@
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="I7" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="J7" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="K7" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L7">
         <v>100</v>
@@ -1623,37 +1632,37 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
       <c r="G8" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="I8" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="J8" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="K8" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="L8">
         <v>10</v>
@@ -1667,37 +1676,37 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
       <c r="G9" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="H9" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="I9" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="J9" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="K9" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="L9">
         <v>10</v>
@@ -1711,257 +1720,257 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>279</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>280</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>281</v>
+      </c>
+      <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
       <c r="G10" t="s">
-        <v>181</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>182</v>
+        <v>282</v>
+      </c>
+      <c r="H10" s="10">
+        <v>824521131</v>
       </c>
       <c r="I10" t="s">
-        <v>183</v>
+        <v>283</v>
       </c>
       <c r="J10" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="K10" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="M10" s="3">
-        <v>0.78100000000000003</v>
+        <v>3.51</v>
       </c>
       <c r="N10" s="3">
-        <v>78.099999999999994</v>
+        <v>70.2</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>278</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="I11" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="J11" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="K11" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L11">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="M11" s="3">
-        <v>4.29</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="N11" s="3">
-        <v>85.8</v>
+        <v>78.099999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="I12" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="J12" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="K12" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L12">
         <v>20</v>
       </c>
       <c r="M12" s="3">
-        <v>3.89</v>
+        <v>4.29</v>
       </c>
       <c r="N12" s="3">
-        <v>77.8</v>
+        <v>85.8</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>284</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="I13" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="J13" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="K13" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M13" s="3">
-        <v>4.6100000000000003</v>
+        <v>3.89</v>
       </c>
       <c r="N13" s="3">
-        <v>46.1</v>
+        <v>77.8</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G14" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="I14" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="J14" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="K14" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="L14">
         <v>10</v>
       </c>
       <c r="M14" s="3">
-        <v>5.8</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="N14" s="3">
-        <v>58</v>
+        <v>46.1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="I15" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="J15" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="K15" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="L15">
         <v>10</v>
@@ -1975,455 +1984,455 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="I16" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="J16" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="K16" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="L16">
         <v>10</v>
       </c>
       <c r="M16" s="3">
-        <v>8.57</v>
+        <v>5.8</v>
       </c>
       <c r="N16" s="3">
-        <v>85.7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="I17" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="J17" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="K17" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M17" s="3">
-        <v>22.74</v>
+        <v>8.57</v>
       </c>
       <c r="N17" s="3">
-        <v>45.48</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="I18" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="J18" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="K18" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="L18">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="M18" s="3">
-        <v>1.32</v>
+        <v>22.74</v>
       </c>
       <c r="N18" s="3">
-        <v>66</v>
+        <v>45.48</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G19" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="I19" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="J19" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="K19" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L19">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="M19" s="3">
-        <v>10.46</v>
+        <v>1.32</v>
       </c>
       <c r="N19" s="3">
-        <v>104.6</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G20" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="I20" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="J20" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="K20" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L20">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="M20" s="3">
-        <v>1.06</v>
+        <v>10.46</v>
       </c>
       <c r="N20" s="3">
-        <v>53</v>
+        <v>104.6</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G21" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="I21" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="J21" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="K21" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L21">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="M21" s="3">
-        <v>27.63</v>
+        <v>1.06</v>
       </c>
       <c r="N21" s="3">
-        <v>110.52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F22" t="s">
-        <v>95</v>
-      </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="G22" t="s">
+        <v>202</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J22" t="s">
+        <v>205</v>
+      </c>
+      <c r="K22" t="s">
+        <v>143</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+      <c r="M22" s="3">
+        <v>27.63</v>
+      </c>
+      <c r="N22" s="3">
+        <v>110.52</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" t="s">
-        <v>220</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="I23" t="s">
-        <v>179</v>
-      </c>
-      <c r="J23" t="s">
-        <v>222</v>
-      </c>
-      <c r="K23" t="s">
-        <v>157</v>
-      </c>
-      <c r="L23">
-        <v>100</v>
-      </c>
-      <c r="M23" s="3">
-        <v>0.77</v>
-      </c>
-      <c r="N23" s="3">
-        <v>77</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" t="s">
+        <v>206</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I24" t="s">
+        <v>165</v>
+      </c>
+      <c r="J24" t="s">
+        <v>208</v>
+      </c>
+      <c r="K24" t="s">
+        <v>143</v>
+      </c>
+      <c r="L24">
         <v>100</v>
       </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" t="s">
-        <v>223</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="I24" t="s">
-        <v>225</v>
-      </c>
-      <c r="J24" t="s">
-        <v>226</v>
-      </c>
-      <c r="K24" t="s">
-        <v>176</v>
-      </c>
-      <c r="L24">
-        <v>1000</v>
-      </c>
       <c r="M24" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.77</v>
       </c>
       <c r="N24" s="3">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="I25" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="J25" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="K25" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="L25">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="M25" s="3">
-        <v>0.128</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="N25" s="3">
-        <v>12.8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>289</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G26" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="I26" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="J26" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="K26" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="L26">
         <v>100</v>
@@ -2437,37 +2446,37 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>286</v>
       </c>
       <c r="B27">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>285</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F27" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="I27" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="J27" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="K27" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="L27">
         <v>100</v>
@@ -2481,37 +2490,37 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>287</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G28" t="s">
-        <v>236</v>
-      </c>
-      <c r="H28" t="s">
-        <v>237</v>
+        <v>216</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="I28" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="J28" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="K28" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="L28">
         <v>100</v>
@@ -2525,459 +2534,525 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>288</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="F29" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="I29" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="J29" t="s">
-        <v>242</v>
+        <v>221</v>
+      </c>
+      <c r="K29" t="s">
+        <v>162</v>
       </c>
       <c r="L29">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="M29" s="3">
-        <v>7.39</v>
+        <v>0.128</v>
       </c>
       <c r="N29" s="3">
-        <v>73.900000000000006</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="E30" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F30" t="s">
-        <v>122</v>
-      </c>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="G30" t="s">
+        <v>222</v>
+      </c>
+      <c r="H30" t="s">
+        <v>223</v>
+      </c>
+      <c r="I30" t="s">
+        <v>211</v>
+      </c>
+      <c r="J30" t="s">
+        <v>224</v>
+      </c>
+      <c r="K30" t="s">
+        <v>162</v>
+      </c>
+      <c r="L30">
+        <v>100</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0.128</v>
+      </c>
+      <c r="N30" s="3">
+        <v>12.8</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>275</v>
       </c>
       <c r="D31" t="s">
-        <v>275</v>
+        <v>106</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="F31" t="s">
-        <v>276</v>
+        <v>108</v>
       </c>
       <c r="G31" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="I31" t="s">
-        <v>270</v>
+        <v>227</v>
       </c>
       <c r="J31" t="s">
-        <v>271</v>
-      </c>
-      <c r="K31" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="L31">
-        <v>20</v>
-      </c>
-      <c r="M31" s="5">
-        <v>5.28</v>
-      </c>
-      <c r="N31" s="5">
-        <v>105.6</v>
+        <v>10</v>
+      </c>
+      <c r="M31" s="3">
+        <v>7.39</v>
+      </c>
+      <c r="N31" s="3">
+        <v>73.900000000000006</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>261</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="F32" t="s">
-        <v>132</v>
+        <v>262</v>
       </c>
       <c r="G32" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="I32" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="J32" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="K32" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L32">
-        <v>5</v>
-      </c>
-      <c r="M32" s="3">
-        <v>31.37</v>
-      </c>
-      <c r="N32" s="3">
-        <v>156.85</v>
+        <v>20</v>
+      </c>
+      <c r="M32" s="5">
+        <v>5.28</v>
+      </c>
+      <c r="N32" s="5">
+        <v>105.6</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F33" t="s">
-        <v>127</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="L33" s="6">
-        <v>10</v>
-      </c>
-      <c r="M33" s="7">
-        <v>5.28</v>
-      </c>
-      <c r="N33" s="7">
-        <v>52.8</v>
+        <v>118</v>
+      </c>
+      <c r="G33" t="s">
+        <v>229</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I33" t="s">
+        <v>231</v>
+      </c>
+      <c r="J33" t="s">
+        <v>232</v>
+      </c>
+      <c r="K33" t="s">
+        <v>143</v>
+      </c>
+      <c r="L33">
+        <v>5</v>
+      </c>
+      <c r="M33" s="3">
+        <v>31.37</v>
+      </c>
+      <c r="N33" s="3">
+        <v>156.85</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="E34" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="F34" t="s">
-        <v>138</v>
-      </c>
-      <c r="G34" t="s">
-        <v>247</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="I34" t="s">
-        <v>245</v>
-      </c>
-      <c r="J34" t="s">
-        <v>249</v>
-      </c>
-      <c r="K34" t="s">
-        <v>157</v>
-      </c>
-      <c r="L34">
-        <v>3</v>
-      </c>
-      <c r="M34" s="3">
-        <v>116.48</v>
-      </c>
-      <c r="N34" s="3">
-        <v>349.44</v>
+        <v>113</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="L34" s="6">
+        <v>10</v>
+      </c>
+      <c r="M34" s="7">
+        <v>5.28</v>
+      </c>
+      <c r="N34" s="7">
+        <v>52.8</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="D35" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="E35" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="F35" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="G35" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="I35" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="J35" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="K35" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L35">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M35" s="3">
-        <v>8.91</v>
+        <v>116.48</v>
       </c>
       <c r="N35" s="3">
-        <v>89.1</v>
+        <v>349.44</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="F36" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="G36" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="I36" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="J36" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="K36" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L36">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M36" s="3">
-        <v>39.409999999999997</v>
+        <v>8.91</v>
       </c>
       <c r="N36" s="3">
-        <v>197.05</v>
+        <v>89.1</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E37" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="F37" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="G37" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="I37" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="J37" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="K37" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L37">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M37" s="3">
-        <v>3.84</v>
+        <v>39.409999999999997</v>
       </c>
       <c r="N37" s="3">
-        <v>38.4</v>
+        <v>197.05</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>277</v>
+        <v>134</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>279</v>
+      <c r="C38" t="s">
+        <v>135</v>
       </c>
       <c r="D38" t="s">
-        <v>282</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="G38" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="L38" s="8">
-        <v>2</v>
-      </c>
-      <c r="M38" s="9">
-        <v>47.81</v>
-      </c>
-      <c r="N38" s="9">
-        <v>95.62</v>
+        <v>135</v>
+      </c>
+      <c r="E38" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" t="s">
+        <v>137</v>
+      </c>
+      <c r="G38" t="s">
+        <v>244</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="I38" t="s">
+        <v>238</v>
+      </c>
+      <c r="J38" t="s">
+        <v>246</v>
+      </c>
+      <c r="K38" t="s">
+        <v>143</v>
+      </c>
+      <c r="L38">
+        <v>10</v>
+      </c>
+      <c r="M38" s="3">
+        <v>3.84</v>
+      </c>
+      <c r="N38" s="3">
+        <v>38.4</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>263</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>284</v>
+      <c r="C39" s="8" t="s">
+        <v>265</v>
       </c>
       <c r="D39" t="s">
-        <v>287</v>
-      </c>
-      <c r="G39" t="s">
-        <v>283</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="I39" t="s">
-        <v>285</v>
-      </c>
-      <c r="J39" t="s">
-        <v>286</v>
-      </c>
-      <c r="L39">
+        <v>268</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="G39" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L39" s="8">
+        <v>2</v>
+      </c>
+      <c r="M39" s="9">
+        <v>47.81</v>
+      </c>
+      <c r="N39" s="9">
+        <v>95.62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40">
         <v>1</v>
       </c>
-      <c r="M39" s="2">
+      <c r="C40" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D40" t="s">
+        <v>273</v>
+      </c>
+      <c r="G40" t="s">
+        <v>269</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="I40" t="s">
+        <v>271</v>
+      </c>
+      <c r="J40" t="s">
+        <v>272</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40" s="2">
         <v>61.33</v>
       </c>
-      <c r="N39" s="5">
+      <c r="N40" s="5">
         <v>61.33</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H43" s="2"/>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
     </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update BOM with price per assembly
</commit_message>
<xml_diff>
--- a/bom/door_bell.xlsx
+++ b/bom/door_bell.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/espen/Projects/KiCad/projects/dual-button-doorbell/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8884B0AA-CC99-DC44-AA49-41085B95DBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C83F6A-152B-DE4C-8280-E12DA956D25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1220" windowWidth="33600" windowHeight="17440" xr2:uid="{3EF4FAFF-71C4-2545-A4EC-35E72D213441}"/>
+    <workbookView xWindow="37580" yWindow="3400" windowWidth="62760" windowHeight="22620" xr2:uid="{3EF4FAFF-71C4-2545-A4EC-35E72D213441}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="292">
   <si>
     <t>Ref</t>
   </si>
@@ -906,6 +906,12 @@
   </si>
   <si>
     <t>R3, R4, R9, R10, R13, R18, R19, R20, R21, R22</t>
+  </si>
+  <si>
+    <t>Production cost</t>
+  </si>
+  <si>
+    <t>(eBay)</t>
   </si>
 </sst>
 </file>
@@ -966,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -984,6 +990,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1300,13 +1308,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E0BB35-FFD4-EE4A-92C0-E7A191100E0E}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" customWidth="1"/>
+    <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="34.5" customWidth="1"/>
@@ -1320,9 +1328,10 @@
     <col min="12" max="12" width="10.5" customWidth="1"/>
     <col min="13" max="13" width="12.83203125" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1365,8 +1374,11 @@
       <c r="N1" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1409,8 +1421,12 @@
       <c r="N2" s="3">
         <v>152.69999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="11">
+        <f>B2*M2</f>
+        <v>15.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1453,8 +1469,12 @@
       <c r="N3" s="3">
         <v>32.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3" s="11">
+        <f t="shared" ref="O3:O40" si="0">B3*M3</f>
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>277</v>
       </c>
@@ -1497,8 +1517,12 @@
       <c r="N4" s="3">
         <v>32.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="11">
+        <f t="shared" si="0"/>
+        <v>1.304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>276</v>
       </c>
@@ -1541,8 +1565,12 @@
       <c r="N5" s="3">
         <v>98.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="11">
+        <f t="shared" si="0"/>
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1585,8 +1613,12 @@
       <c r="N6" s="3">
         <v>44.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="11">
+        <f t="shared" si="0"/>
+        <v>0.443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1629,8 +1661,12 @@
       <c r="N7" s="3">
         <v>26.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0720000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1673,8 +1709,12 @@
       <c r="N8" s="3">
         <v>47.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="11">
+        <f t="shared" si="0"/>
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1717,8 +1757,12 @@
       <c r="N9" s="3">
         <v>32.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="11">
+        <f t="shared" si="0"/>
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -1761,8 +1805,12 @@
       <c r="N10" s="3">
         <v>70.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="11">
+        <f t="shared" si="0"/>
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>278</v>
       </c>
@@ -1805,8 +1853,12 @@
       <c r="N11" s="3">
         <v>78.099999999999994</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="11">
+        <f t="shared" si="0"/>
+        <v>5.4670000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1849,8 +1901,12 @@
       <c r="N12" s="3">
         <v>85.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="11">
+        <f t="shared" si="0"/>
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>284</v>
       </c>
@@ -1893,8 +1949,12 @@
       <c r="N13" s="3">
         <v>77.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="11">
+        <f t="shared" si="0"/>
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1937,8 +1997,12 @@
       <c r="N14" s="3">
         <v>46.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="11">
+        <f t="shared" si="0"/>
+        <v>4.6100000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1981,8 +2045,12 @@
       <c r="N15" s="3">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="11">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -2025,8 +2093,12 @@
       <c r="N16" s="3">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="11">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2069,8 +2141,12 @@
       <c r="N17" s="3">
         <v>85.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="11">
+        <f t="shared" si="0"/>
+        <v>8.57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -2113,8 +2189,12 @@
       <c r="N18" s="3">
         <v>45.48</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="11">
+        <f t="shared" si="0"/>
+        <v>22.74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -2157,8 +2237,12 @@
       <c r="N19" s="3">
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="11">
+        <f t="shared" si="0"/>
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -2201,8 +2285,12 @@
       <c r="N20" s="3">
         <v>104.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="11">
+        <f t="shared" si="0"/>
+        <v>10.46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -2245,8 +2333,12 @@
       <c r="N21" s="3">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="11">
+        <f t="shared" si="0"/>
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -2289,8 +2381,12 @@
       <c r="N22" s="3">
         <v>110.52</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="11">
+        <f t="shared" si="0"/>
+        <v>27.63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -2309,10 +2405,24 @@
       <c r="F23" t="s">
         <v>91</v>
       </c>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>291</v>
+      </c>
+      <c r="L23">
+        <v>50</v>
+      </c>
+      <c r="M23" s="4">
+        <v>8.9</v>
+      </c>
+      <c r="N23" s="4">
+        <v>445</v>
+      </c>
+      <c r="O23" s="11">
+        <f t="shared" si="0"/>
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -2355,8 +2465,12 @@
       <c r="N24" s="3">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24" s="11">
+        <f t="shared" si="0"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -2399,8 +2513,12 @@
       <c r="N25" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25" s="11">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>289</v>
       </c>
@@ -2443,8 +2561,12 @@
       <c r="N26" s="3">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26" s="11">
+        <f t="shared" si="0"/>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>286</v>
       </c>
@@ -2487,8 +2609,12 @@
       <c r="N27" s="3">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27" s="11">
+        <f t="shared" si="0"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>287</v>
       </c>
@@ -2531,8 +2657,12 @@
       <c r="N28" s="3">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="11">
+        <f t="shared" si="0"/>
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>288</v>
       </c>
@@ -2575,8 +2705,12 @@
       <c r="N29" s="3">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" s="11">
+        <f t="shared" si="0"/>
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -2619,8 +2753,12 @@
       <c r="N30" s="3">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30" s="11">
+        <f t="shared" si="0"/>
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>274</v>
       </c>
@@ -2660,8 +2798,12 @@
       <c r="N31" s="3">
         <v>73.900000000000006</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31" s="11">
+        <f t="shared" si="0"/>
+        <v>14.78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>109</v>
       </c>
@@ -2703,6 +2845,10 @@
       </c>
       <c r="N32" s="5">
         <v>105.6</v>
+      </c>
+      <c r="O32" s="11">
+        <f t="shared" si="0"/>
+        <v>5.28</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
@@ -2748,6 +2894,10 @@
       <c r="N33" s="3">
         <v>156.85</v>
       </c>
+      <c r="O33" s="11">
+        <f t="shared" si="0"/>
+        <v>31.37</v>
+      </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -2792,6 +2942,10 @@
       <c r="N34" s="7">
         <v>52.8</v>
       </c>
+      <c r="O34" s="11">
+        <f t="shared" si="0"/>
+        <v>5.28</v>
+      </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -2836,6 +2990,10 @@
       <c r="N35" s="3">
         <v>349.44</v>
       </c>
+      <c r="O35" s="11">
+        <f t="shared" si="0"/>
+        <v>116.48</v>
+      </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -2880,6 +3038,10 @@
       <c r="N36" s="3">
         <v>89.1</v>
       </c>
+      <c r="O36" s="11">
+        <f t="shared" si="0"/>
+        <v>8.91</v>
+      </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -2924,6 +3086,10 @@
       <c r="N37" s="3">
         <v>197.05</v>
       </c>
+      <c r="O37" s="11">
+        <f t="shared" si="0"/>
+        <v>39.409999999999997</v>
+      </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -2968,6 +3134,10 @@
       <c r="N38" s="3">
         <v>38.4</v>
       </c>
+      <c r="O38" s="11">
+        <f t="shared" si="0"/>
+        <v>3.84</v>
+      </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -3007,6 +3177,10 @@
       <c r="N39" s="9">
         <v>95.62</v>
       </c>
+      <c r="O39" s="11">
+        <f t="shared" si="0"/>
+        <v>47.81</v>
+      </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -3041,6 +3215,16 @@
       </c>
       <c r="N40" s="5">
         <v>61.33</v>
+      </c>
+      <c r="O40" s="11">
+        <f t="shared" si="0"/>
+        <v>61.33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O41" s="12">
+        <f>SUM(O2:O40)</f>
+        <v>501.08199999999994</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>